<commit_message>
brand wise api done
</commit_message>
<xml_diff>
--- a/sheetFolder/sheet3.xlsx
+++ b/sheetFolder/sheet3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\PROGRAMS\Mern_Stack Projects\Internship\DataCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8A0E6BB-2847-4985-A5AD-AF250F3DB2A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBDAF927-8FCA-4AB9-9950-E7306E9AE963}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E7850BFF-8745-46CB-BAB3-F48C7D724E5C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="102">
   <si>
     <t>EMPID</t>
   </si>
@@ -277,6 +277,66 @@
   </si>
   <si>
     <t>CONTINUING</t>
+  </si>
+  <si>
+    <t>Amit Kumar Singh</t>
+  </si>
+  <si>
+    <t>E57012</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>SUKRIT SUD</t>
+  </si>
+  <si>
+    <t>`0000592766</t>
+  </si>
+  <si>
+    <t>GAURAV SETH</t>
+  </si>
+  <si>
+    <t>`0001495156</t>
+  </si>
+  <si>
+    <t>PROMILA SHRESTHA</t>
+  </si>
+  <si>
+    <t>BHARTI DEVI</t>
+  </si>
+  <si>
+    <t>ROHIT</t>
+  </si>
+  <si>
+    <t>GAURAV</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>BIHAR</t>
+  </si>
+  <si>
+    <t>HISAR</t>
+  </si>
+  <si>
+    <t>UC</t>
+  </si>
+  <si>
+    <t>MONY ISSUE</t>
+  </si>
+  <si>
+    <t>TOFASHINE</t>
+  </si>
+  <si>
+    <t>HEADON</t>
+  </si>
+  <si>
+    <t>Ravi Pandey</t>
+  </si>
+  <si>
+    <t>E77033</t>
   </si>
 </sst>
 </file>
@@ -393,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -426,6 +486,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -740,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{010365CA-1E6C-4661-AC2E-55C5379C1C58}">
-  <dimension ref="A1:AM5"/>
+  <dimension ref="A1:AM9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AF7" sqref="AF7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,13 +822,15 @@
     <col min="14" max="14" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.5703125" customWidth="1"/>
     <col min="19" max="19" width="13" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" customWidth="1"/>
+    <col min="20" max="20" width="18" customWidth="1"/>
     <col min="23" max="23" width="13.85546875" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" customWidth="1"/>
     <col min="26" max="26" width="14" customWidth="1"/>
     <col min="27" max="27" width="14.42578125" customWidth="1"/>
     <col min="30" max="30" width="15.5703125" customWidth="1"/>
     <col min="33" max="33" width="15.5703125" customWidth="1"/>
     <col min="34" max="34" width="23.42578125" customWidth="1"/>
+    <col min="35" max="35" width="13" customWidth="1"/>
     <col min="36" max="36" width="19" customWidth="1"/>
     <col min="37" max="37" width="15.42578125" customWidth="1"/>
     <col min="39" max="39" width="13.28515625" customWidth="1"/>
@@ -1141,7 +1204,7 @@
         <v>40</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>42</v>
@@ -1260,7 +1323,7 @@
         <v>40</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>42</v>
@@ -1365,6 +1428,482 @@
         <v>63</v>
       </c>
       <c r="AM5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="7">
+        <v>12345</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>3</v>
+      </c>
+      <c r="R6" s="7">
+        <v>10000</v>
+      </c>
+      <c r="S6" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="T6" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="U6" s="9">
+        <v>41</v>
+      </c>
+      <c r="V6" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="W6" s="9">
+        <v>9958272550</v>
+      </c>
+      <c r="X6" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA6" s="8">
+        <v>3</v>
+      </c>
+      <c r="AB6" s="8">
+        <v>14567</v>
+      </c>
+      <c r="AC6" s="8">
+        <v>12</v>
+      </c>
+      <c r="AD6" s="8">
+        <v>5</v>
+      </c>
+      <c r="AE6" s="8">
+        <v>11</v>
+      </c>
+      <c r="AF6" s="8">
+        <v>2020</v>
+      </c>
+      <c r="AG6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI6" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AJ6">
+        <v>6</v>
+      </c>
+      <c r="AK6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="7">
+        <v>12345</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>3</v>
+      </c>
+      <c r="R7" s="7">
+        <v>10000</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="T7" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="U7" s="9">
+        <v>46</v>
+      </c>
+      <c r="V7" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="W7" s="9">
+        <v>9199189658</v>
+      </c>
+      <c r="X7" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y7" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA7" s="8">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="8">
+        <v>12800</v>
+      </c>
+      <c r="AC7" s="8">
+        <v>43</v>
+      </c>
+      <c r="AD7" s="8">
+        <v>4</v>
+      </c>
+      <c r="AE7" s="8">
+        <v>12</v>
+      </c>
+      <c r="AF7" s="8">
+        <v>2020</v>
+      </c>
+      <c r="AG7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH7" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI7" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AJ7">
+        <v>5</v>
+      </c>
+      <c r="AK7" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="7">
+        <v>12345</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>4</v>
+      </c>
+      <c r="R8" s="7">
+        <v>40000</v>
+      </c>
+      <c r="S8" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="T8" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="U8" s="8">
+        <v>48</v>
+      </c>
+      <c r="V8" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="W8" s="8">
+        <v>7960708132</v>
+      </c>
+      <c r="X8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z8" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA8" s="8">
+        <v>3</v>
+      </c>
+      <c r="AB8" s="8">
+        <v>12800</v>
+      </c>
+      <c r="AC8" s="8">
+        <v>15</v>
+      </c>
+      <c r="AD8" s="8">
+        <v>9</v>
+      </c>
+      <c r="AE8" s="8">
+        <v>10</v>
+      </c>
+      <c r="AF8" s="8">
+        <v>2020</v>
+      </c>
+      <c r="AG8" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH8" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI8" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="AJ8">
+        <v>4</v>
+      </c>
+      <c r="AK8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="7">
+        <v>12345</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>4</v>
+      </c>
+      <c r="R9" s="7">
+        <v>40000</v>
+      </c>
+      <c r="S9" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="T9" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U9" s="8">
+        <v>46</v>
+      </c>
+      <c r="V9" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="W9" s="8">
+        <v>9680515160</v>
+      </c>
+      <c r="X9" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y9" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z9" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA9" s="8">
+        <v>3</v>
+      </c>
+      <c r="AB9" s="8">
+        <v>12800</v>
+      </c>
+      <c r="AC9" s="8">
+        <v>10</v>
+      </c>
+      <c r="AD9" s="8">
+        <v>3</v>
+      </c>
+      <c r="AE9" s="8">
+        <v>10</v>
+      </c>
+      <c r="AF9" s="8">
+        <v>2020</v>
+      </c>
+      <c r="AG9" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH9" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI9" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="AJ9">
+        <v>3</v>
+      </c>
+      <c r="AK9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM9" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>